<commit_message>
fixed slopes for log transformed variables
</commit_message>
<xml_diff>
--- a/Analysis/tables/Narea_model.xlsx
+++ b/Analysis/tables/Narea_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/NutNetPhys/Analysis/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08649D64-32F6-9B4D-AC63-2FF994572F0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C176F1-5B34-E646-8AC8-50435D9B0703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15480" yWindow="3940" windowWidth="21400" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15680" yWindow="4260" windowWidth="21400" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Narea_model" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>Var</t>
   </si>
@@ -86,8 +86,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -566,10 +568,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -925,18 +928,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,7 +955,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -969,7 +972,7 @@
       <c r="D2" s="1">
         <v>4.0637758695073099E-57</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1.00002654377168</v>
       </c>
     </row>
@@ -986,7 +989,7 @@
       <c r="D3" s="1">
         <v>0.72611097454542195</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>0.116827614873448</v>
       </c>
     </row>
@@ -1003,7 +1006,7 @@
       <c r="D4" s="1">
         <v>0.48931331627374403</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>0.115577525396998</v>
       </c>
     </row>
@@ -1020,7 +1023,7 @@
       <c r="D5" s="1">
         <v>2.12347089533153E-2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>5.3880686539834199</v>
       </c>
     </row>
@@ -1037,7 +1040,7 @@
       <c r="D6" s="1">
         <v>2.95406972238711E-2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>4.68713118264768</v>
       </c>
     </row>
@@ -1046,15 +1049,15 @@
         <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>-1.4255117150092201E-4</v>
+        <v>-0.114992084861493</v>
       </c>
       <c r="C7" s="1">
-        <v>3.5422179455519101E-4</v>
+        <v>0.285740918369213</v>
       </c>
       <c r="D7" s="1">
         <v>0.68445733170647005</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>19.379221598948501</v>
       </c>
     </row>
@@ -1063,15 +1066,15 @@
         <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>-6.0027808921401797E-2</v>
+        <v>-3.3297323192085997E-2</v>
       </c>
       <c r="C8" s="1">
-        <v>0.154508815207581</v>
+        <v>8.5705776179994406E-2</v>
       </c>
       <c r="D8" s="1">
         <v>0.69578031483158798</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>2.3634848313246399</v>
       </c>
     </row>
@@ -1079,16 +1082,16 @@
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>6.6979409268331394E-5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>6.87385248351198E-5</v>
       </c>
       <c r="D9" s="1">
         <v>0.32692041627075402</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>2.9271551094463</v>
       </c>
     </row>
@@ -1097,15 +1100,15 @@
         <v>12</v>
       </c>
       <c r="B10" s="1">
-        <v>7.0185830549187602E-4</v>
+        <v>0.93553292553719403</v>
       </c>
       <c r="C10" s="1">
-        <v>6.5803647248791398E-6</v>
+        <v>8.7712118158288204E-3</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>53.031856166271801</v>
       </c>
     </row>
@@ -1122,7 +1125,7 @@
       <c r="D11" s="1">
         <v>1.0767283375713999E-16</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>5.0380713231964798</v>
       </c>
     </row>
@@ -1139,7 +1142,7 @@
       <c r="D12" s="1">
         <v>2.6783608733173601E-9</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>3.68074729272338</v>
       </c>
     </row>
@@ -1156,8 +1159,8 @@
       <c r="D13" s="1">
         <v>3.4560546415596501E-3</v>
       </c>
-      <c r="E13" s="2">
-        <v>0.40150894289661399</v>
+      <c r="E13" s="1">
+        <v>0.13414764901703899</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1173,8 +1176,8 @@
       <c r="D14" s="1">
         <v>0.578322567132036</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>4</v>
+      <c r="E14" s="1">
+        <v>0.149452310426681</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1190,8 +1193,8 @@
       <c r="D15" s="1">
         <v>0.767149080866947</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>4</v>
+      <c r="E15" s="1">
+        <v>4.8506400071264201E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1207,12 +1210,9 @@
       <c r="D16" s="1">
         <v>0.89809327826557495</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="2"/>
+      <c r="E16" s="1">
+        <v>6.9402583381629704E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fixed issues with figs & tables
</commit_message>
<xml_diff>
--- a/Analysis/tables/Narea_model.xlsx
+++ b/Analysis/tables/Narea_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/risa/Git/NutNetPhys/Analysis/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C176F1-5B34-E646-8AC8-50435D9B0703}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2E1846-02C5-F842-9C98-BAFAEEF07855}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15680" yWindow="4260" windowWidth="21400" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13060" yWindow="500" windowWidth="21400" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Narea_model" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>SE</t>
   </si>
   <si>
-    <t>RelImp</t>
+    <t>Relative Importance</t>
   </si>
 </sst>
 </file>
@@ -568,11 +568,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -931,7 +932,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,7 +940,7 @@
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -972,7 +973,7 @@
       <c r="D2" s="1">
         <v>4.0637758695073099E-57</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <v>1.00002654377168</v>
       </c>
     </row>
@@ -989,7 +990,7 @@
       <c r="D3" s="1">
         <v>0.72611097454542195</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="4">
         <v>0.116827614873448</v>
       </c>
     </row>
@@ -1006,7 +1007,7 @@
       <c r="D4" s="1">
         <v>0.48931331627374403</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>0.115577525396998</v>
       </c>
     </row>
@@ -1023,7 +1024,7 @@
       <c r="D5" s="1">
         <v>2.12347089533153E-2</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>5.3880686539834199</v>
       </c>
     </row>
@@ -1040,7 +1041,7 @@
       <c r="D6" s="1">
         <v>2.95406972238711E-2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="4">
         <v>4.68713118264768</v>
       </c>
     </row>
@@ -1057,7 +1058,7 @@
       <c r="D7" s="1">
         <v>0.68445733170647005</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="4">
         <v>19.379221598948501</v>
       </c>
     </row>
@@ -1074,7 +1075,7 @@
       <c r="D8" s="1">
         <v>0.69578031483158798</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="4">
         <v>2.3634848313246399</v>
       </c>
     </row>
@@ -1091,7 +1092,7 @@
       <c r="D9" s="1">
         <v>0.32692041627075402</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="4">
         <v>2.9271551094463</v>
       </c>
     </row>
@@ -1108,7 +1109,7 @@
       <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>53.031856166271801</v>
       </c>
     </row>
@@ -1125,7 +1126,7 @@
       <c r="D11" s="1">
         <v>1.0767283375713999E-16</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="4">
         <v>5.0380713231964798</v>
       </c>
     </row>
@@ -1142,7 +1143,7 @@
       <c r="D12" s="1">
         <v>2.6783608733173601E-9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="4">
         <v>3.68074729272338</v>
       </c>
     </row>
@@ -1159,7 +1160,7 @@
       <c r="D13" s="1">
         <v>3.4560546415596501E-3</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="4">
         <v>0.13414764901703899</v>
       </c>
     </row>
@@ -1176,7 +1177,7 @@
       <c r="D14" s="1">
         <v>0.578322567132036</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="4">
         <v>0.149452310426681</v>
       </c>
     </row>
@@ -1193,7 +1194,7 @@
       <c r="D15" s="1">
         <v>0.767149080866947</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="4">
         <v>4.8506400071264201E-2</v>
       </c>
     </row>
@@ -1210,7 +1211,7 @@
       <c r="D16" s="1">
         <v>0.89809327826557495</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="4">
         <v>6.9402583381629704E-2</v>
       </c>
     </row>

</xml_diff>